<commit_message>
Prints list of movies for user to select
</commit_message>
<xml_diff>
--- a/showtimes.xlsx
+++ b/showtimes.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="64">
   <si>
     <t>Movies Playing</t>
   </si>
@@ -29,214 +29,184 @@
     <t>Release Year</t>
   </si>
   <si>
-    <t>The Predator</t>
+    <t>Venom</t>
+  </si>
+  <si>
+    <t>7.1</t>
+  </si>
+  <si>
+    <t>112</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>A Star Is Born</t>
+  </si>
+  <si>
+    <t>8.5</t>
+  </si>
+  <si>
+    <t>135</t>
+  </si>
+  <si>
+    <t>A Simple Favor</t>
+  </si>
+  <si>
+    <t>7.2</t>
+  </si>
+  <si>
+    <t>117</t>
+  </si>
+  <si>
+    <t>Night School</t>
+  </si>
+  <si>
+    <t>5.5</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>The Nun</t>
+  </si>
+  <si>
+    <t>5.7</t>
+  </si>
+  <si>
+    <t>96</t>
+  </si>
+  <si>
+    <t>Smallfoot</t>
+  </si>
+  <si>
+    <t>6.8</t>
+  </si>
+  <si>
+    <t>The House with a Clock in Its Walls</t>
+  </si>
+  <si>
+    <t>6.3</t>
+  </si>
+  <si>
+    <t>105</t>
+  </si>
+  <si>
+    <t>Mandy</t>
+  </si>
+  <si>
+    <t>121</t>
+  </si>
+  <si>
+    <t>Crazy Rich Asians</t>
+  </si>
+  <si>
+    <t>7.5</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>Hell Fest</t>
   </si>
   <si>
     <t>5.9</t>
   </si>
   <si>
-    <t>107</t>
-  </si>
-  <si>
-    <t>2018</t>
-  </si>
-  <si>
-    <t>A Simple Favor</t>
-  </si>
-  <si>
-    <t>7.2</t>
-  </si>
-  <si>
-    <t>117</t>
-  </si>
-  <si>
-    <t>A Star Is Born</t>
-  </si>
-  <si>
-    <t>8.6</t>
-  </si>
-  <si>
-    <t>135</t>
-  </si>
-  <si>
-    <t>The Nun</t>
-  </si>
-  <si>
-    <t>5.7</t>
-  </si>
-  <si>
-    <t>96</t>
-  </si>
-  <si>
-    <t>The House with a Clock in Its Walls</t>
-  </si>
-  <si>
-    <t>6.3</t>
-  </si>
-  <si>
-    <t>105</t>
-  </si>
-  <si>
-    <t>Mandy</t>
-  </si>
-  <si>
-    <t>6.8</t>
-  </si>
-  <si>
-    <t>121</t>
-  </si>
-  <si>
-    <t>Night School</t>
-  </si>
-  <si>
-    <t>5.5</t>
-  </si>
-  <si>
-    <t>111</t>
-  </si>
-  <si>
-    <t>Crazy Rich Asians</t>
-  </si>
-  <si>
-    <t>7.5</t>
-  </si>
-  <si>
-    <t>120</t>
-  </si>
-  <si>
-    <t>Mission: Impossible - Fallout</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>147</t>
-  </si>
-  <si>
-    <t>Searching</t>
-  </si>
-  <si>
-    <t>7.9</t>
+    <t>89</t>
+  </si>
+  <si>
+    <t>BlacKkKlansman</t>
+  </si>
+  <si>
+    <t>7.8</t>
+  </si>
+  <si>
+    <t>White Boy Rick</t>
+  </si>
+  <si>
+    <t>6.6</t>
+  </si>
+  <si>
+    <t>Assassination Nation</t>
+  </si>
+  <si>
+    <t>108</t>
+  </si>
+  <si>
+    <t>Christopher Robin</t>
+  </si>
+  <si>
+    <t>7.7</t>
+  </si>
+  <si>
+    <t>104</t>
+  </si>
+  <si>
+    <t>Fahrenheit 11/9</t>
+  </si>
+  <si>
+    <t>128</t>
+  </si>
+  <si>
+    <t>The Wife</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>The Little Stranger</t>
+  </si>
+  <si>
+    <t>6.1</t>
+  </si>
+  <si>
+    <t>Ghost Busters</t>
+  </si>
+  <si>
+    <t>1984</t>
+  </si>
+  <si>
+    <t>Kin</t>
+  </si>
+  <si>
+    <t>5.6</t>
   </si>
   <si>
     <t>102</t>
   </si>
   <si>
-    <t>Smallfoot</t>
-  </si>
-  <si>
-    <t>Hell Fest</t>
-  </si>
-  <si>
-    <t>89</t>
-  </si>
-  <si>
-    <t>Peppermint</t>
-  </si>
-  <si>
-    <t>6.6</t>
-  </si>
-  <si>
-    <t>101</t>
-  </si>
-  <si>
-    <t>Life Itself</t>
-  </si>
-  <si>
-    <t>5.8</t>
-  </si>
-  <si>
-    <t>118</t>
-  </si>
-  <si>
-    <t>BlacKkKlansman</t>
-  </si>
-  <si>
-    <t>7.8</t>
-  </si>
-  <si>
-    <t>White Boy Rick</t>
-  </si>
-  <si>
-    <t>Fahrenheit 11/9</t>
-  </si>
-  <si>
-    <t>5.4</t>
-  </si>
-  <si>
-    <t>128</t>
-  </si>
-  <si>
-    <t>Little Italy</t>
-  </si>
-  <si>
-    <t>Little Women</t>
-  </si>
-  <si>
-    <t>4.5</t>
-  </si>
-  <si>
-    <t>112</t>
-  </si>
-  <si>
-    <t>Sorry to Bother You</t>
-  </si>
-  <si>
-    <t>7.4</t>
-  </si>
-  <si>
-    <t>Die Hard</t>
-  </si>
-  <si>
-    <t>8.2</t>
-  </si>
-  <si>
-    <t>132</t>
-  </si>
-  <si>
-    <t>1988</t>
-  </si>
-  <si>
-    <t>Sui Dhaaga: Made in India</t>
-  </si>
-  <si>
-    <t>6.9</t>
-  </si>
-  <si>
-    <t>122</t>
-  </si>
-  <si>
-    <t>Qismat</t>
-  </si>
-  <si>
-    <t>9.4</t>
-  </si>
-  <si>
-    <t>137</t>
-  </si>
-  <si>
-    <t>An Ideal Husband</t>
-  </si>
-  <si>
-    <t>97</t>
-  </si>
-  <si>
-    <t>1999</t>
-  </si>
-  <si>
-    <t>Scotty and the Secret History of Hollywood</t>
+    <t>The Children Act</t>
+  </si>
+  <si>
+    <t>6.7</t>
+  </si>
+  <si>
+    <t>Mary Shelley</t>
   </si>
   <si>
     <t>6.4</t>
   </si>
   <si>
-    <t>98</t>
-  </si>
-  <si>
-    <t>Becoming Burlesque</t>
-  </si>
-  <si>
-    <t>2017</t>
+    <t>The Dawn Wall</t>
+  </si>
+  <si>
+    <t>8.1</t>
+  </si>
+  <si>
+    <t>Hello, Mrs. Money</t>
+  </si>
+  <si>
+    <t>5.3</t>
+  </si>
+  <si>
+    <t>113</t>
+  </si>
+  <si>
+    <t>My Generation</t>
+  </si>
+  <si>
+    <t>85</t>
   </si>
 </sst>
 </file>
@@ -585,7 +555,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -685,7 +655,7 @@
         <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
@@ -693,13 +663,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
@@ -707,13 +677,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
         <v>26</v>
-      </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -721,13 +691,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
         <v>29</v>
-      </c>
-      <c r="B10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" t="s">
-        <v>31</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
@@ -735,13 +705,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
         <v>32</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" t="s">
-        <v>34</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
@@ -749,13 +719,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
@@ -763,13 +733,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
         <v>36</v>
       </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
@@ -777,13 +747,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
         <v>38</v>
-      </c>
-      <c r="B14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" t="s">
-        <v>40</v>
       </c>
       <c r="D14" t="s">
         <v>7</v>
@@ -791,13 +761,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" t="s">
         <v>41</v>
-      </c>
-      <c r="B15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" t="s">
-        <v>43</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
@@ -805,13 +775,13 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
@@ -819,13 +789,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
@@ -833,13 +803,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
         <v>47</v>
       </c>
-      <c r="B18" t="s">
-        <v>48</v>
-      </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
@@ -847,27 +817,27 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" t="s">
         <v>51</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>52</v>
-      </c>
-      <c r="C20" t="s">
-        <v>53</v>
       </c>
       <c r="D20" t="s">
         <v>7</v>
@@ -875,13 +845,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" t="s">
         <v>54</v>
       </c>
-      <c r="B21" t="s">
-        <v>55</v>
-      </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D21" t="s">
         <v>7</v>
@@ -889,27 +859,27 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" t="s">
         <v>56</v>
       </c>
-      <c r="B22" t="s">
-        <v>57</v>
-      </c>
       <c r="C22" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="D22" t="s">
-        <v>59</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B23" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="D23" t="s">
         <v>7</v>
@@ -917,13 +887,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B24" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C24" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D24" t="s">
         <v>7</v>
@@ -931,44 +901,16 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B25" t="s">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="C25" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D25" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" t="s">
-        <v>69</v>
-      </c>
-      <c r="B26" t="s">
-        <v>70</v>
-      </c>
-      <c r="C26" t="s">
-        <v>71</v>
-      </c>
-      <c r="D26" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" t="s">
-        <v>72</v>
-      </c>
-      <c r="B27" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Scapred genre and audience rating of the movie
Stores all the scapped information for each movie and imporved the formating of the printed lists
</commit_message>
<xml_diff>
--- a/showtimes.xlsx
+++ b/showtimes.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="68">
   <si>
     <t>Movies Playing</t>
   </si>
@@ -92,12 +92,6 @@
     <t>105</t>
   </si>
   <si>
-    <t>Mandy</t>
-  </si>
-  <si>
-    <t>121</t>
-  </si>
-  <si>
     <t>Crazy Rich Asians</t>
   </si>
   <si>
@@ -128,10 +122,13 @@
     <t>6.6</t>
   </si>
   <si>
-    <t>Assassination Nation</t>
-  </si>
-  <si>
-    <t>108</t>
+    <t>Mamma Mia! Here We Go Again</t>
+  </si>
+  <si>
+    <t>114</t>
+  </si>
+  <si>
+    <t>Boku no Hero Academia the Movie</t>
   </si>
   <si>
     <t>Christopher Robin</t>
@@ -155,37 +152,34 @@
     <t>100</t>
   </si>
   <si>
+    <t>Sui Dhaaga: Made in India</t>
+  </si>
+  <si>
+    <t>6.9</t>
+  </si>
+  <si>
+    <t>122</t>
+  </si>
+  <si>
     <t>The Little Stranger</t>
   </si>
   <si>
     <t>6.1</t>
   </si>
   <si>
-    <t>Ghost Busters</t>
-  </si>
-  <si>
-    <t>1984</t>
-  </si>
-  <si>
-    <t>Kin</t>
-  </si>
-  <si>
-    <t>5.6</t>
-  </si>
-  <si>
-    <t>102</t>
-  </si>
-  <si>
     <t>The Children Act</t>
   </si>
   <si>
     <t>6.7</t>
   </si>
   <si>
-    <t>Mary Shelley</t>
-  </si>
-  <si>
-    <t>6.4</t>
+    <t>Qismat</t>
+  </si>
+  <si>
+    <t>9.4</t>
+  </si>
+  <si>
+    <t>137</t>
   </si>
   <si>
     <t>The Dawn Wall</t>
@@ -203,10 +197,28 @@
     <t>113</t>
   </si>
   <si>
+    <t>Kusama: Infinity</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
     <t>My Generation</t>
   </si>
   <si>
     <t>85</t>
+  </si>
+  <si>
+    <t>Afsar</t>
+  </si>
+  <si>
+    <t>127</t>
+  </si>
+  <si>
+    <t>The Woman Who Fell to Earth</t>
+  </si>
+  <si>
+    <t>60</t>
   </si>
 </sst>
 </file>
@@ -555,7 +567,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -680,10 +692,10 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -691,13 +703,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
@@ -705,13 +717,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
@@ -725,7 +737,7 @@
         <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
@@ -736,10 +748,10 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
         <v>36</v>
-      </c>
-      <c r="C13" t="s">
-        <v>16</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
@@ -750,10 +762,10 @@
         <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s">
         <v>7</v>
@@ -761,13 +773,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
         <v>39</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>40</v>
-      </c>
-      <c r="C15" t="s">
-        <v>41</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
@@ -775,13 +787,13 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
@@ -789,13 +801,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
         <v>44</v>
-      </c>
-      <c r="B17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" t="s">
-        <v>45</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
@@ -803,13 +815,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
         <v>46</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>47</v>
-      </c>
-      <c r="C18" t="s">
-        <v>16</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
@@ -820,13 +832,13 @@
         <v>48</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -837,7 +849,7 @@
         <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="D20" t="s">
         <v>7</v>
@@ -845,13 +857,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" t="s">
         <v>53</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>54</v>
-      </c>
-      <c r="C21" t="s">
-        <v>24</v>
       </c>
       <c r="D21" t="s">
         <v>7</v>
@@ -865,7 +877,7 @@
         <v>56</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="D22" t="s">
         <v>7</v>
@@ -879,7 +891,7 @@
         <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="D23" t="s">
         <v>7</v>
@@ -887,10 +899,10 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="C24" t="s">
         <v>61</v>
@@ -910,6 +922,34 @@
         <v>63</v>
       </c>
       <c r="D25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Prompts user input to select a movie
created get_selection() helper function and a while loop to ensure a valid input
</commit_message>
<xml_diff>
--- a/showtimes.xlsx
+++ b/showtimes.xlsx
@@ -161,16 +161,16 @@
     <t>122</t>
   </si>
   <si>
+    <t>The Children Act</t>
+  </si>
+  <si>
+    <t>6.7</t>
+  </si>
+  <si>
     <t>The Little Stranger</t>
   </si>
   <si>
     <t>6.1</t>
-  </si>
-  <si>
-    <t>The Children Act</t>
-  </si>
-  <si>
-    <t>6.7</t>
   </si>
   <si>
     <t>Qismat</t>
@@ -835,7 +835,7 @@
         <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
@@ -849,7 +849,7 @@
         <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D20" t="s">
         <v>7</v>
@@ -930,7 +930,7 @@
         <v>64</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C26" t="s">
         <v>65</v>

</xml_diff>

<commit_message>
Created new soup of the selected movie using URL processing
</commit_message>
<xml_diff>
--- a/showtimes.xlsx
+++ b/showtimes.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="69">
   <si>
     <t>Movies Playing</t>
   </si>
@@ -210,6 +210,9 @@
   </si>
   <si>
     <t>Afsar</t>
+  </si>
+  <si>
+    <t>6.4</t>
   </si>
   <si>
     <t>127</t>
@@ -916,7 +919,7 @@
         <v>62</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C25" t="s">
         <v>63</v>
@@ -930,10 +933,10 @@
         <v>64</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="C26" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D26" t="s">
         <v>7</v>
@@ -941,13 +944,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C27" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D27" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Added feature to allow users to input custom postal code
</commit_message>
<xml_diff>
--- a/showtimes.xlsx
+++ b/showtimes.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="98">
   <si>
     <t>Movies Playing</t>
   </si>
@@ -29,199 +29,286 @@
     <t>Release Year</t>
   </si>
   <si>
+    <t>Halloween</t>
+  </si>
+  <si>
+    <t>7.5</t>
+  </si>
+  <si>
+    <t>106</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>A Star Is Born</t>
+  </si>
+  <si>
+    <t>8.3</t>
+  </si>
+  <si>
+    <t>136</t>
+  </si>
+  <si>
     <t>Venom</t>
   </si>
   <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>112</t>
+  </si>
+  <si>
+    <t>First Man</t>
+  </si>
+  <si>
+    <t>7.7</t>
+  </si>
+  <si>
+    <t>141</t>
+  </si>
+  <si>
+    <t>Bad Times at the El Royale</t>
+  </si>
+  <si>
+    <t>7.8</t>
+  </si>
+  <si>
+    <t>91</t>
+  </si>
+  <si>
+    <t>1978</t>
+  </si>
+  <si>
+    <t>Ant-Man and the Wasp</t>
+  </si>
+  <si>
+    <t>7.2</t>
+  </si>
+  <si>
+    <t>118</t>
+  </si>
+  <si>
+    <t>Goosebumps 2: Haunted Halloween</t>
+  </si>
+  <si>
+    <t>6.1</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>A Simple Favor</t>
+  </si>
+  <si>
     <t>7.1</t>
   </si>
   <si>
-    <t>112</t>
-  </si>
-  <si>
-    <t>2018</t>
-  </si>
-  <si>
-    <t>A Star Is Born</t>
+    <t>117</t>
+  </si>
+  <si>
+    <t>The Nun</t>
+  </si>
+  <si>
+    <t>5.7</t>
+  </si>
+  <si>
+    <t>96</t>
+  </si>
+  <si>
+    <t>Night School</t>
+  </si>
+  <si>
+    <t>5.5</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>The Hate U Give</t>
+  </si>
+  <si>
+    <t>6.4</t>
+  </si>
+  <si>
+    <t>133</t>
+  </si>
+  <si>
+    <t>The Predator</t>
+  </si>
+  <si>
+    <t>5.9</t>
+  </si>
+  <si>
+    <t>107</t>
+  </si>
+  <si>
+    <t>The Meg</t>
+  </si>
+  <si>
+    <t>113</t>
+  </si>
+  <si>
+    <t>Smallfoot</t>
+  </si>
+  <si>
+    <t>6.8</t>
+  </si>
+  <si>
+    <t>The House with a Clock in Its Walls</t>
+  </si>
+  <si>
+    <t>6.2</t>
+  </si>
+  <si>
+    <t>105</t>
+  </si>
+  <si>
+    <t>Crazy Rich Asians</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>Incredibles 2</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>The Sisters Brothers</t>
+  </si>
+  <si>
+    <t>121</t>
+  </si>
+  <si>
+    <t>Peppermint</t>
+  </si>
+  <si>
+    <t>6.6</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>Colette</t>
+  </si>
+  <si>
+    <t>6.9</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>Badhaai Ho</t>
+  </si>
+  <si>
+    <t>8.4</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>Namaste England</t>
+  </si>
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t>The New Romantic</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>Mo seung</t>
+  </si>
+  <si>
+    <t>7.3</t>
+  </si>
+  <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>Exes Baggage</t>
+  </si>
+  <si>
+    <t>104</t>
+  </si>
+  <si>
+    <t>Qismat</t>
+  </si>
+  <si>
+    <t>9.3</t>
+  </si>
+  <si>
+    <t>137</t>
+  </si>
+  <si>
+    <t>Son of Manjeet Singh</t>
   </si>
   <si>
     <t>8.5</t>
   </si>
   <si>
-    <t>135</t>
-  </si>
-  <si>
-    <t>A Simple Favor</t>
-  </si>
-  <si>
-    <t>7.2</t>
-  </si>
-  <si>
-    <t>117</t>
-  </si>
-  <si>
-    <t>Night School</t>
-  </si>
-  <si>
-    <t>5.5</t>
-  </si>
-  <si>
-    <t>111</t>
-  </si>
-  <si>
-    <t>The Nun</t>
-  </si>
-  <si>
-    <t>5.7</t>
-  </si>
-  <si>
-    <t>96</t>
-  </si>
-  <si>
-    <t>Smallfoot</t>
-  </si>
-  <si>
-    <t>6.8</t>
-  </si>
-  <si>
-    <t>The House with a Clock in Its Walls</t>
-  </si>
-  <si>
-    <t>6.3</t>
-  </si>
-  <si>
-    <t>105</t>
-  </si>
-  <si>
-    <t>Crazy Rich Asians</t>
-  </si>
-  <si>
-    <t>7.5</t>
-  </si>
-  <si>
-    <t>120</t>
-  </si>
-  <si>
-    <t>Hell Fest</t>
-  </si>
-  <si>
-    <t>5.9</t>
-  </si>
-  <si>
-    <t>89</t>
-  </si>
-  <si>
-    <t>BlacKkKlansman</t>
-  </si>
-  <si>
-    <t>7.8</t>
-  </si>
-  <si>
-    <t>White Boy Rick</t>
-  </si>
-  <si>
-    <t>6.6</t>
-  </si>
-  <si>
-    <t>Mamma Mia! Here We Go Again</t>
-  </si>
-  <si>
-    <t>114</t>
-  </si>
-  <si>
-    <t>Boku no Hero Academia the Movie</t>
-  </si>
-  <si>
-    <t>Christopher Robin</t>
-  </si>
-  <si>
-    <t>7.7</t>
-  </si>
-  <si>
-    <t>104</t>
-  </si>
-  <si>
-    <t>Fahrenheit 11/9</t>
-  </si>
-  <si>
-    <t>128</t>
-  </si>
-  <si>
-    <t>The Wife</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>Sui Dhaaga: Made in India</t>
-  </si>
-  <si>
-    <t>6.9</t>
-  </si>
-  <si>
-    <t>122</t>
-  </si>
-  <si>
-    <t>The Children Act</t>
-  </si>
-  <si>
-    <t>6.7</t>
-  </si>
-  <si>
-    <t>The Little Stranger</t>
-  </si>
-  <si>
-    <t>6.1</t>
-  </si>
-  <si>
-    <t>Qismat</t>
-  </si>
-  <si>
-    <t>9.4</t>
-  </si>
-  <si>
-    <t>137</t>
-  </si>
-  <si>
-    <t>The Dawn Wall</t>
-  </si>
-  <si>
-    <t>8.1</t>
-  </si>
-  <si>
-    <t>Hello, Mrs. Money</t>
-  </si>
-  <si>
-    <t>5.3</t>
-  </si>
-  <si>
-    <t>113</t>
-  </si>
-  <si>
-    <t>Kusama: Infinity</t>
-  </si>
-  <si>
-    <t>76</t>
-  </si>
-  <si>
-    <t>My Generation</t>
-  </si>
-  <si>
-    <t>85</t>
+    <t>139</t>
+  </si>
+  <si>
+    <t>Sharkwater Extinction</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>Aate di chidi</t>
+  </si>
+  <si>
+    <t>140</t>
   </si>
   <si>
     <t>Afsar</t>
   </si>
   <si>
-    <t>6.4</t>
-  </si>
-  <si>
     <t>127</t>
   </si>
   <si>
-    <t>The Woman Who Fell to Earth</t>
-  </si>
-  <si>
-    <t>60</t>
+    <t>Space Station 3D</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>2002</t>
+  </si>
+  <si>
+    <t>Deep Sea</t>
+  </si>
+  <si>
+    <t>7.6</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>2006</t>
+  </si>
+  <si>
+    <t>Bugs!</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>2003</t>
+  </si>
+  <si>
+    <t>Galapagos: Nature's Wonderland</t>
+  </si>
+  <si>
+    <t>2014</t>
   </si>
 </sst>
 </file>
@@ -570,7 +657,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -653,10 +740,10 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -664,27 +751,27 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>23</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
@@ -692,13 +779,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
         <v>25</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>26</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -706,13 +793,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
         <v>28</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>29</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
@@ -720,13 +807,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
         <v>31</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>32</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
@@ -740,7 +827,7 @@
         <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
@@ -748,13 +835,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
@@ -762,13 +849,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
         <v>7</v>
@@ -776,13 +863,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
@@ -790,13 +877,13 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
@@ -804,13 +891,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
@@ -818,13 +905,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
@@ -832,13 +919,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
@@ -846,13 +933,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="D20" t="s">
         <v>7</v>
@@ -860,13 +947,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C21" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D21" t="s">
         <v>7</v>
@@ -874,27 +961,27 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D22" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D23" t="s">
         <v>7</v>
@@ -902,13 +989,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="D24" t="s">
         <v>7</v>
@@ -916,13 +1003,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D25" t="s">
         <v>7</v>
@@ -930,13 +1017,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C26" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D26" t="s">
         <v>7</v>
@@ -944,16 +1031,142 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="C27" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D27" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>84</v>
+      </c>
+      <c r="B32" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>86</v>
+      </c>
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>89</v>
+      </c>
+      <c r="B34" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>93</v>
+      </c>
+      <c r="B35" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" t="s">
+        <v>94</v>
+      </c>
+      <c r="D35" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>96</v>
+      </c>
+      <c r="B36" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" t="s">
+        <v>94</v>
+      </c>
+      <c r="D36" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>